<commit_message>
setting up vennegruppe on a new computer
</commit_message>
<xml_diff>
--- a/groups.xlsx
+++ b/groups.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vennegruppe" sheetId="1" state="visible" r:id="rId1"/>
@@ -388,75 +388,75 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0"/>
-    <xf borderId="9" fillId="6" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="16" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="10" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="24" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="10" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="19" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="20" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="22" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="1"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="2"/>
-    <cellStyle builtinId="10" name="Note" xfId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
+    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -769,7 +769,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="6" min="1" style="14" width="14"/>
+    <col width="14" bestFit="1" customWidth="1" style="14" min="1" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -801,30 +801,30 @@
       <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="2" s="14">
+    <row r="2" ht="15" customHeight="1" s="14">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hermine</t>
+          <t>Ria</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Klara</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Penny</t>
+          <t>Abel</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Klara</t>
+          <t>Ulu</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Benni</t>
+          <t>Iris</t>
         </is>
       </c>
       <c r="N2" s="2" t="n"/>
@@ -833,20 +833,20 @@
       <c r="Q2" s="2" t="n"/>
       <c r="R2" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="3" s="14">
+    <row r="3" ht="15" customHeight="1" s="14">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ulu</t>
+          <t>Vance</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Abel</t>
+          <t>Dora</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Wyatt</t>
+          <t>Lars</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>Fransy</t>
         </is>
       </c>
       <c r="N3" s="2" t="n"/>
@@ -865,30 +865,30 @@
       <c r="Q3" s="2" t="n"/>
       <c r="R3" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4" s="14">
+    <row r="4" ht="15" customHeight="1" s="14">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ede</t>
+          <t>Penny</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lars</t>
+          <t>Maya</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ria</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Benni</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Olav</t>
+          <t>Stan</t>
         </is>
       </c>
       <c r="N4" s="2" t="n"/>
@@ -897,30 +897,30 @@
       <c r="Q4" s="2" t="n"/>
       <c r="R4" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="5" s="14">
+    <row r="5" ht="15" customHeight="1" s="14">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dora</t>
+          <t>Wyatt</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Stan</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Iris</t>
+          <t>Gert</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Vance</t>
+          <t>Ede</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="N5" s="2" t="n"/>
@@ -929,20 +929,20 @@
       <c r="Q5" s="2" t="n"/>
       <c r="R5" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6" s="14">
+    <row r="6" ht="15" customHeight="1" s="14">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Maya</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gert</t>
+          <t>Hermine</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fransy</t>
+          <t>Olav</t>
         </is>
       </c>
       <c r="N6" s="2" t="n"/>
@@ -951,14 +951,14 @@
       <c r="Q6" s="2" t="n"/>
       <c r="R6" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15.6" r="7" s="14" thickBot="1">
+    <row r="7" ht="15.6" customHeight="1" s="14" thickBot="1">
       <c r="N7" s="2" t="n"/>
       <c r="O7" s="2" t="n"/>
       <c r="P7" s="2" t="n"/>
       <c r="Q7" s="2" t="n"/>
       <c r="R7" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="8" s="14">
+    <row r="8" ht="15" customHeight="1" s="14">
       <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Hvis du bruker denne appen for første gang, men klassen har allerede hatt en eller flere vennegrupper:</t>
@@ -985,7 +985,7 @@
       <c r="Q8" s="2" t="n"/>
       <c r="R8" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="9" s="14">
+    <row r="9" ht="15" customHeight="1" s="14">
       <c r="A9" s="13" t="n"/>
       <c r="E9" s="15" t="n"/>
       <c r="G9" s="13" t="n"/>
@@ -996,7 +996,7 @@
       <c r="Q9" s="2" t="n"/>
       <c r="R9" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="10" s="14">
+    <row r="10" ht="15" customHeight="1" s="14">
       <c r="A10" s="27" t="n"/>
       <c r="B10" s="20" t="n"/>
       <c r="C10" s="20" t="n"/>
@@ -1015,7 +1015,7 @@
       <c r="Q10" s="2" t="n"/>
       <c r="R10" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11" s="14">
+    <row r="11" ht="15" customHeight="1" s="14">
       <c r="A11" s="16" t="inlineStr">
         <is>
           <t>Skriv in siste Vennegrupper overfor. Viktig! Endre overskrivt 'Vennegruppe x' til riktig antal grupper.</t>
@@ -1037,7 +1037,7 @@
       <c r="Q11" s="2" t="n"/>
       <c r="R11" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12" s="14">
+    <row r="12" ht="15" customHeight="1" s="14">
       <c r="A12" s="19" t="n"/>
       <c r="B12" s="20" t="n"/>
       <c r="C12" s="20" t="n"/>
@@ -1051,7 +1051,7 @@
       <c r="Q12" s="2" t="n"/>
       <c r="R12" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13" s="14">
+    <row r="13" ht="15" customHeight="1" s="14">
       <c r="A13" s="24" t="n"/>
       <c r="B13" s="25" t="n"/>
       <c r="C13" s="25" t="n"/>
@@ -1070,7 +1070,7 @@
       <c r="Q13" s="2" t="n"/>
       <c r="R13" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14" s="14" thickBot="1">
+    <row r="14" ht="15" customHeight="1" s="14" thickBot="1">
       <c r="A14" s="22" t="inlineStr">
         <is>
           <t>Når du får dette dokument etter bruk av appen, her er de nyeste vennegrupper notert for deg. Bruk den dokumet igjen når du skal lage nye grupper.</t>
@@ -1092,7 +1092,7 @@
       <c r="Q14" s="2" t="n"/>
       <c r="R14" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15.6" r="15" s="14" thickBot="1">
+    <row r="15" ht="15.6" customHeight="1" s="14" thickBot="1">
       <c r="A15" s="19" t="n"/>
       <c r="B15" s="20" t="n"/>
       <c r="C15" s="20" t="n"/>
@@ -1110,63 +1110,63 @@
       <c r="P15" s="2" t="n"/>
       <c r="Q15" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16" s="14">
+    <row r="16" ht="15" customHeight="1" s="14">
       <c r="N16" s="2" t="n"/>
       <c r="O16" s="2" t="n"/>
       <c r="P16" s="2" t="n"/>
       <c r="Q16" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17" s="14">
+    <row r="17" ht="15" customHeight="1" s="14">
       <c r="N17" s="2" t="n"/>
       <c r="O17" s="2" t="n"/>
       <c r="P17" s="2" t="n"/>
       <c r="Q17" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18" s="14">
+    <row r="18" ht="15" customHeight="1" s="14">
       <c r="N18" s="2" t="n"/>
       <c r="O18" s="2" t="n"/>
       <c r="P18" s="2" t="n"/>
       <c r="Q18" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19" s="14">
+    <row r="19" ht="15" customHeight="1" s="14">
       <c r="N19" s="2" t="n"/>
       <c r="O19" s="2" t="n"/>
       <c r="P19" s="2" t="n"/>
       <c r="Q19" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="20" s="14">
+    <row r="20" ht="15" customHeight="1" s="14">
       <c r="N20" s="2" t="n"/>
       <c r="O20" s="2" t="n"/>
       <c r="P20" s="2" t="n"/>
       <c r="Q20" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="21" s="14">
+    <row r="21" ht="15" customHeight="1" s="14">
       <c r="N21" s="2" t="n"/>
       <c r="O21" s="2" t="n"/>
       <c r="P21" s="2" t="n"/>
       <c r="Q21" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22" s="14">
+    <row r="22" ht="15" customHeight="1" s="14">
       <c r="N22" s="2" t="n"/>
       <c r="O22" s="2" t="n"/>
       <c r="P22" s="2" t="n"/>
       <c r="Q22" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="23" s="14">
+    <row r="23" ht="15" customHeight="1" s="14">
       <c r="N23" s="2" t="n"/>
       <c r="O23" s="2" t="n"/>
       <c r="P23" s="2" t="n"/>
       <c r="Q23" s="2" t="n"/>
       <c r="R23" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24" s="14">
+    <row r="24" ht="15" customHeight="1" s="14">
       <c r="N24" s="2" t="n"/>
       <c r="O24" s="2" t="n"/>
       <c r="P24" s="2" t="n"/>
       <c r="Q24" s="2" t="n"/>
       <c r="R24" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25" s="14">
+    <row r="25" ht="15" customHeight="1" s="14">
       <c r="N25" s="2" t="n"/>
       <c r="O25" s="2" t="n"/>
       <c r="P25" s="2" t="n"/>
@@ -1184,7 +1184,7 @@
     <mergeCell ref="G11:M12"/>
     <mergeCell ref="G14:M15"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -1195,7 +1195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T153"/>
+  <dimension ref="A1:V153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
@@ -1238,7 +1238,7 @@
       <c r="A3" s="13" t="n"/>
       <c r="T3" s="15" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="4" s="14" thickBot="1">
+    <row r="4" ht="15" customHeight="1" s="14" thickBot="1">
       <c r="A4" s="31" t="n"/>
       <c r="B4" s="32" t="n"/>
       <c r="C4" s="32" t="n"/>
@@ -1280,7 +1280,7 @@
       <c r="E5" s="4" t="n"/>
       <c r="F5" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="6" s="14">
+    <row r="6" ht="15" customHeight="1" s="14">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Abel</t>
@@ -1346,8 +1346,48 @@
           <t>Stan</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="14">
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="14">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Benni</t>
@@ -1408,8 +1448,43 @@
           <t>Q</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="8" s="14">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="14">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Chris</t>
@@ -1480,8 +1555,38 @@
           <t>Hermine</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="14">
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="14">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Dora</t>
@@ -1552,8 +1657,48 @@
           <t>Hermine</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="10" s="14">
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="14">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Ede</t>
@@ -1624,8 +1769,48 @@
           <t>Penny</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="11" s="14">
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="14">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Fransy</t>
@@ -1691,8 +1876,43 @@
           <t>Maya</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="12" s="14">
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="14">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Gert</t>
@@ -1763,8 +1983,48 @@
           <t>Stan</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="13" s="14">
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="14">
       <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Hermine</t>
@@ -1830,8 +2090,48 @@
           <t>Dora</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="14" s="14">
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Iris</t>
@@ -1902,8 +2202,43 @@
           <t>Penny</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="15" s="14">
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="14">
       <c r="A15" s="2" t="inlineStr">
         <is>
           <t>John</t>
@@ -1974,8 +2309,43 @@
           <t>Stan</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="16" s="14">
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="14">
       <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Klara</t>
@@ -2036,8 +2406,43 @@
           <t>Fransy</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="17" s="14">
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" s="14">
       <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Lars</t>
@@ -2108,8 +2513,48 @@
           <t>Hermine</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="18" s="14">
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" s="14">
       <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Maya</t>
@@ -2170,8 +2615,43 @@
           <t>Fransy</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="19" s="14">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Ulu</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" s="14">
       <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Nick</t>
@@ -2237,8 +2717,43 @@
           <t>Stan</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="20" s="14">
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1" s="14">
       <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Olav</t>
@@ -2304,8 +2819,38 @@
           <t>Penny</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="21" s="14">
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" s="14">
       <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Penny</t>
@@ -2366,8 +2911,48 @@
           <t>Ede</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="22" s="14">
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" s="14">
       <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Q</t>
@@ -2423,8 +3008,43 @@
           <t>Wyatt</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="23" s="14">
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1" s="14">
       <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Ria</t>
@@ -2485,8 +3105,48 @@
           <t>Penny</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="24" s="14">
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Wyatt</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Stan</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1" s="14">
       <c r="A24" s="2" t="inlineStr">
         <is>
           <t>Stan</t>
@@ -2552,8 +3212,48 @@
           <t>Gert</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="25" s="14">
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Benni</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" s="14">
       <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Tanya</t>
@@ -2614,8 +3314,38 @@
           <t>Fransy</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="26" s="14">
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Vance</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" s="14">
       <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Ulu</t>
@@ -2681,8 +3411,48 @@
           <t>Hermine</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="27" s="14">
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Maya</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Dora</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Gert</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Ede</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Hermine</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="14">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Vance</t>
@@ -2748,8 +3518,43 @@
           <t>Q</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="28" s="14">
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Klara</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Tanya</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Lars</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Abel</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Nick</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" s="14">
       <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Wyatt</t>
@@ -2815,383 +3620,418 @@
           <t>Q</t>
         </is>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="30" s="14">
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Penny</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Ria</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Iris</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Fransy</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>Olav</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" s="14">
       <c r="B30" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="31" s="14">
+    <row r="31" ht="15" customHeight="1" s="14">
       <c r="B31" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="32" s="14">
+    <row r="32" ht="15" customHeight="1" s="14">
       <c r="B32" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="33" s="14">
+    <row r="33" ht="15" customHeight="1" s="14">
       <c r="B33" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="34" s="14">
+    <row r="34" ht="15" customHeight="1" s="14">
       <c r="B34" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="35" s="14">
+    <row r="35" ht="15" customHeight="1" s="14">
       <c r="B35" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="36" s="14">
+    <row r="36" ht="15" customHeight="1" s="14">
       <c r="B36" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="37" s="14">
+    <row r="37" ht="15" customHeight="1" s="14">
       <c r="B37" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="38" s="14">
+    <row r="38" ht="15" customHeight="1" s="14">
       <c r="B38" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="39" s="14">
+    <row r="39" ht="15" customHeight="1" s="14">
       <c r="B39" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="40" s="14">
+    <row r="40" ht="15" customHeight="1" s="14">
       <c r="B40" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="41" s="14">
+    <row r="41" ht="15" customHeight="1" s="14">
       <c r="B41" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="42" s="14">
+    <row r="42" ht="15" customHeight="1" s="14">
       <c r="B42" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="43" s="14">
+    <row r="43" ht="15" customHeight="1" s="14">
       <c r="B43" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="44" s="14">
+    <row r="44" ht="15" customHeight="1" s="14">
       <c r="B44" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="45" s="14">
+    <row r="45" ht="15" customHeight="1" s="14">
       <c r="B45" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="46" s="14">
+    <row r="46" ht="15" customHeight="1" s="14">
       <c r="B46" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="47" s="14">
+    <row r="47" ht="15" customHeight="1" s="14">
       <c r="B47" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="48" s="14">
+    <row r="48" ht="15" customHeight="1" s="14">
       <c r="B48" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="49" s="14">
+    <row r="49" ht="15" customHeight="1" s="14">
       <c r="B49" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="50" s="14">
+    <row r="50" ht="15" customHeight="1" s="14">
       <c r="B50" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="51" s="14">
+    <row r="51" ht="15" customHeight="1" s="14">
       <c r="B51" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="52" s="14">
+    <row r="52" ht="15" customHeight="1" s="14">
       <c r="B52" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="53" s="14">
+    <row r="53" ht="15" customHeight="1" s="14">
       <c r="B53" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="54" s="14">
+    <row r="54" ht="15" customHeight="1" s="14">
       <c r="B54" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="55" s="14">
+    <row r="55" ht="15" customHeight="1" s="14">
       <c r="B55" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="56" s="14">
+    <row r="56" ht="15" customHeight="1" s="14">
       <c r="B56" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="57" s="14">
+    <row r="57" ht="15" customHeight="1" s="14">
       <c r="B57" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="58" s="14">
+    <row r="58" ht="15" customHeight="1" s="14">
       <c r="B58" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="59" s="14">
+    <row r="59" ht="15" customHeight="1" s="14">
       <c r="B59" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="60" s="14">
+    <row r="60" ht="15" customHeight="1" s="14">
       <c r="B60" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="61" s="14">
+    <row r="61" ht="15" customHeight="1" s="14">
       <c r="B61" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="62" s="14">
+    <row r="62" ht="15" customHeight="1" s="14">
       <c r="B62" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="63" s="14">
+    <row r="63" ht="15" customHeight="1" s="14">
       <c r="B63" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="64" s="14">
+    <row r="64" ht="15" customHeight="1" s="14">
       <c r="B64" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="65" s="14">
+    <row r="65" ht="15" customHeight="1" s="14">
       <c r="B65" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="66" s="14">
+    <row r="66" ht="15" customHeight="1" s="14">
       <c r="B66" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="67" s="14">
+    <row r="67" ht="15" customHeight="1" s="14">
       <c r="B67" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="68" s="14">
+    <row r="68" ht="15" customHeight="1" s="14">
       <c r="B68" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="69" s="14">
+    <row r="69" ht="15" customHeight="1" s="14">
       <c r="B69" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="70" s="14">
+    <row r="70" ht="15" customHeight="1" s="14">
       <c r="B70" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="71" s="14">
+    <row r="71" ht="15" customHeight="1" s="14">
       <c r="B71" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="72" s="14">
+    <row r="72" ht="15" customHeight="1" s="14">
       <c r="B72" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="73" s="14">
+    <row r="73" ht="15" customHeight="1" s="14">
       <c r="B73" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="74" s="14">
+    <row r="74" ht="15" customHeight="1" s="14">
       <c r="B74" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="75" s="14">
+    <row r="75" ht="15" customHeight="1" s="14">
       <c r="B75" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="76" s="14">
+    <row r="76" ht="15" customHeight="1" s="14">
       <c r="B76" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="77" s="14">
+    <row r="77" ht="15" customHeight="1" s="14">
       <c r="B77" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="78" s="14">
+    <row r="78" ht="15" customHeight="1" s="14">
       <c r="B78" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="79" s="14">
+    <row r="79" ht="15" customHeight="1" s="14">
       <c r="B79" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="80" s="14">
+    <row r="80" ht="15" customHeight="1" s="14">
       <c r="B80" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="81" s="14">
+    <row r="81" ht="15" customHeight="1" s="14">
       <c r="B81" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="82" s="14">
+    <row r="82" ht="15" customHeight="1" s="14">
       <c r="B82" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="83" s="14">
+    <row r="83" ht="15" customHeight="1" s="14">
       <c r="B83" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="84" s="14">
+    <row r="84" ht="15" customHeight="1" s="14">
       <c r="B84" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="85" s="14">
+    <row r="85" ht="15" customHeight="1" s="14">
       <c r="B85" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="86" s="14">
+    <row r="86" ht="15" customHeight="1" s="14">
       <c r="B86" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="87" s="14">
+    <row r="87" ht="15" customHeight="1" s="14">
       <c r="B87" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="88" s="14">
+    <row r="88" ht="15" customHeight="1" s="14">
       <c r="B88" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="89" s="14">
+    <row r="89" ht="15" customHeight="1" s="14">
       <c r="B89" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="90" s="14">
+    <row r="90" ht="15" customHeight="1" s="14">
       <c r="B90" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="91" s="14">
+    <row r="91" ht="15" customHeight="1" s="14">
       <c r="B91" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="92" s="14">
+    <row r="92" ht="15" customHeight="1" s="14">
       <c r="B92" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="93" s="14">
+    <row r="93" ht="15" customHeight="1" s="14">
       <c r="B93" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="94" s="14">
+    <row r="94" ht="15" customHeight="1" s="14">
       <c r="B94" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="95" s="14">
+    <row r="95" ht="15" customHeight="1" s="14">
       <c r="B95" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="96" s="14">
+    <row r="96" ht="15" customHeight="1" s="14">
       <c r="B96" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="97" s="14">
+    <row r="97" ht="15" customHeight="1" s="14">
       <c r="B97" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="98" s="14">
+    <row r="98" ht="15" customHeight="1" s="14">
       <c r="B98" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="99" s="14">
+    <row r="99" ht="15" customHeight="1" s="14">
       <c r="B99" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="100" s="14">
+    <row r="100" ht="15" customHeight="1" s="14">
       <c r="B100" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="101" s="14">
+    <row r="101" ht="15" customHeight="1" s="14">
       <c r="B101" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="102" s="14">
+    <row r="102" ht="15" customHeight="1" s="14">
       <c r="B102" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="103" s="14">
+    <row r="103" ht="15" customHeight="1" s="14">
       <c r="B103" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="104" s="14">
+    <row r="104" ht="15" customHeight="1" s="14">
       <c r="B104" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="105" s="14">
+    <row r="105" ht="15" customHeight="1" s="14">
       <c r="B105" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="106" s="14">
+    <row r="106" ht="15" customHeight="1" s="14">
       <c r="B106" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="107" s="14">
+    <row r="107" ht="15" customHeight="1" s="14">
       <c r="B107" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="108" s="14">
+    <row r="108" ht="15" customHeight="1" s="14">
       <c r="B108" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="109" s="14">
+    <row r="109" ht="15" customHeight="1" s="14">
       <c r="B109" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="110" s="14">
+    <row r="110" ht="15" customHeight="1" s="14">
       <c r="B110" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="111" s="14">
+    <row r="111" ht="15" customHeight="1" s="14">
       <c r="B111" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="112" s="14">
+    <row r="112" ht="15" customHeight="1" s="14">
       <c r="B112" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="113" s="14">
+    <row r="113" ht="15" customHeight="1" s="14">
       <c r="B113" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="114" s="14">
+    <row r="114" ht="15" customHeight="1" s="14">
       <c r="B114" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="115" s="14">
+    <row r="115" ht="15" customHeight="1" s="14">
       <c r="B115" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="116" s="14">
+    <row r="116" ht="15" customHeight="1" s="14">
       <c r="B116" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="117" s="14">
+    <row r="117" ht="15" customHeight="1" s="14">
       <c r="B117" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="118" s="14">
+    <row r="118" ht="15" customHeight="1" s="14">
       <c r="B118" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="119" s="14">
+    <row r="119" ht="15" customHeight="1" s="14">
       <c r="B119" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="120" s="14">
+    <row r="120" ht="15" customHeight="1" s="14">
       <c r="B120" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="121" s="14">
+    <row r="121" ht="15" customHeight="1" s="14">
       <c r="B121" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="122" s="14">
+    <row r="122" ht="15" customHeight="1" s="14">
       <c r="B122" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="123" s="14">
+    <row r="123" ht="15" customHeight="1" s="14">
       <c r="B123" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="124" s="14">
+    <row r="124" ht="15" customHeight="1" s="14">
       <c r="B124" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="125" s="14">
+    <row r="125" ht="15" customHeight="1" s="14">
       <c r="B125" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="126" s="14">
+    <row r="126" ht="15" customHeight="1" s="14">
       <c r="B126" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="127" s="14">
+    <row r="127" ht="15" customHeight="1" s="14">
       <c r="B127" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="128" s="14">
+    <row r="128" ht="15" customHeight="1" s="14">
       <c r="B128" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="129" s="14">
+    <row r="129" ht="15" customHeight="1" s="14">
       <c r="B129" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="130" s="14">
+    <row r="130" ht="15" customHeight="1" s="14">
       <c r="B130" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="131" s="14">
+    <row r="131" ht="15" customHeight="1" s="14">
       <c r="B131" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="132" s="14">
+    <row r="132" ht="15" customHeight="1" s="14">
       <c r="B132" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="133" s="14">
+    <row r="133" ht="15" customHeight="1" s="14">
       <c r="B133" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="134" s="14">
+    <row r="134" ht="15" customHeight="1" s="14">
       <c r="B134" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="135" s="14">
+    <row r="135" ht="15" customHeight="1" s="14">
       <c r="B135" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="136" s="14">
+    <row r="136" ht="15" customHeight="1" s="14">
       <c r="B136" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="137" s="14">
+    <row r="137" ht="15" customHeight="1" s="14">
       <c r="B137" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="138" s="14">
+    <row r="138" ht="15" customHeight="1" s="14">
       <c r="B138" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="139" s="14">
+    <row r="139" ht="15" customHeight="1" s="14">
       <c r="B139" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="140" s="14">
+    <row r="140" ht="15" customHeight="1" s="14">
       <c r="B140" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="141" s="14">
+    <row r="141" ht="15" customHeight="1" s="14">
       <c r="B141" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="142" s="14">
+    <row r="142" ht="15" customHeight="1" s="14">
       <c r="B142" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="143" s="14">
+    <row r="143" ht="15" customHeight="1" s="14">
       <c r="B143" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="144" s="14">
+    <row r="144" ht="15" customHeight="1" s="14">
       <c r="B144" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="145" s="14">
+    <row r="145" ht="15" customHeight="1" s="14">
       <c r="B145" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="146" s="14">
+    <row r="146" ht="15" customHeight="1" s="14">
       <c r="B146" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="147" s="14">
+    <row r="147" ht="15" customHeight="1" s="14">
       <c r="B147" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="148" s="14">
+    <row r="148" ht="15" customHeight="1" s="14">
       <c r="B148" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="149" s="14">
+    <row r="149" ht="15" customHeight="1" s="14">
       <c r="B149" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="150" s="14">
+    <row r="150" ht="15" customHeight="1" s="14">
       <c r="B150" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="151" s="14">
+    <row r="151" ht="15" customHeight="1" s="14">
       <c r="B151" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="152" s="14">
+    <row r="152" ht="15" customHeight="1" s="14">
       <c r="B152" s="2" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="153" s="14">
+    <row r="153" ht="15" customHeight="1" s="14">
       <c r="B153" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:T4"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>